<commit_message>
Updated timesheet with info on what was worked on
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -26,12 +26,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>DATE</t>
   </si>
   <si>
     <t>Time Spent (hours)</t>
+  </si>
+  <si>
+    <t>What I worked on</t>
+  </si>
+  <si>
+    <t>Tutorials + implementation for Random map Gen</t>
+  </si>
+  <si>
+    <t>Implementation of Random Map Gen + Player programming</t>
   </si>
 </sst>
 </file>
@@ -39,8 +48,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yy/mm/dd;@"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="yy/mm/dd;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -82,9 +91,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,90 +374,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>42291</v>
       </c>
       <c r="B2" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>42292</v>
       </c>
       <c r="B3" s="4">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
@@ -542,84 +561,88 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B35"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
@@ -718,10 +741,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B32"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,71 +753,74 @@
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>

</xml_diff>

<commit_message>
Updated timesheet plus added missing prefab objects from last commit
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>DATE</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Added Exit sign to map in random room</t>
+  </si>
+  <si>
+    <t>Added random enemy spawning</t>
   </si>
 </sst>
 </file>
@@ -380,7 +383,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,8 +438,15 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="3">
+        <v>42295</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>

</xml_diff>

<commit_message>
Minor Cleanup + TimeSheet
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Provencher" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>DATE</t>
   </si>
@@ -51,11 +51,14 @@
   <si>
     <t>Put work into enemy movement logic and gameobject communication</t>
   </si>
+  <si>
+    <t>Drastically improved enemy spawning + enemy has flying AI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yy/mm/dd;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -386,17 +389,17 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>42291</v>
       </c>
@@ -418,7 +421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>42292</v>
       </c>
@@ -429,7 +432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>42294</v>
       </c>
@@ -440,7 +443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>42295</v>
       </c>
@@ -451,7 +454,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>42297</v>
       </c>
@@ -462,131 +465,138 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>42299</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
     </row>
@@ -604,9 +614,9 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,151 +627,151 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
     </row>
@@ -778,13 +788,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -795,179 +805,179 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added team meeting discussions and minutes
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -12,9 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
-    <sheet name="Provencher" sheetId="1" r:id="rId1"/>
-    <sheet name="Philippona" sheetId="2" r:id="rId2"/>
-    <sheet name="Ningge" sheetId="3" r:id="rId3"/>
+    <sheet name="Team Meetings" sheetId="4" r:id="rId1"/>
+    <sheet name="Provencher" sheetId="1" r:id="rId2"/>
+    <sheet name="Philippona" sheetId="2" r:id="rId3"/>
+    <sheet name="Ningge" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>DATE</t>
   </si>
@@ -62,6 +63,45 @@
   </si>
   <si>
     <t>Fixed crawler enemy animator + added damage from bullet generated</t>
+  </si>
+  <si>
+    <t>Team Discussions</t>
+  </si>
+  <si>
+    <t>Initial project discussion. Idea for proceduraly generated game. 3D RPG</t>
+  </si>
+  <si>
+    <t>Scrapped ambitions for 3D game, decided on 2D procedural generation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussed story, art and inspirations for game. </t>
+  </si>
+  <si>
+    <t>Game Proposal Presentation</t>
+  </si>
+  <si>
+    <t>Discussion on task splitting and implementation details.</t>
+  </si>
+  <si>
+    <t>Online discussion on map creation.</t>
+  </si>
+  <si>
+    <t>Online discussion on player control</t>
+  </si>
+  <si>
+    <t>Online discussion on enemy types</t>
+  </si>
+  <si>
+    <t>Online collaborative trouble shooting on various issues.</t>
+  </si>
+  <si>
+    <t>Discussion on remaining tasks and issues</t>
+  </si>
+  <si>
+    <t>Setting up of online repository and issue tracker establishment</t>
+  </si>
+  <si>
+    <t>Playtesting and discussion of glitches and mechanic improvement ideas</t>
   </si>
 </sst>
 </file>
@@ -109,12 +149,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,10 +436,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>42262</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>42265</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>42267</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>42269</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>42276</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>42291</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>42292</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>42295</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>42297</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>42300</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>42301</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -636,7 +874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
@@ -810,7 +1048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C47"/>
   <sheetViews>

</xml_diff>

<commit_message>
write what I'v done in timesheet
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eprov\Documents\GitHub\TalosOrigins\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team Meetings" sheetId="4" r:id="rId1"/>
@@ -17,7 +12,10 @@
     <sheet name="Philippona" sheetId="2" r:id="rId3"/>
     <sheet name="Ningge" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>DATE</t>
   </si>
@@ -108,12 +106,21 @@
   </si>
   <si>
     <t>Online discussion on Gameplay mechanics</t>
+  </si>
+  <si>
+    <t>Change Talos bullet to particle</t>
+  </si>
+  <si>
+    <t>Add crawler enemy + Crawler animations + crawler bullet animations + crawler shoot bullet towards Talos</t>
+  </si>
+  <si>
+    <t>Talos animations + Talos controls + Talos bullet animations + Talos shoot bullet to the position where the left button of the mouse being pressed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yy/mm/dd;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -164,10 +171,38 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -434,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -444,14 +479,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -649,7 +684,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,14 +1107,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="152.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1094,16 +1130,37 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="3">
+        <v>42299</v>
+      </c>
+      <c r="B2" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="3">
+        <v>42300</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="3">
+        <v>42302</v>
+      </c>
+      <c r="B4" s="4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>

</xml_diff>